<commit_message>
Updated Simulator App test cases
</commit_message>
<xml_diff>
--- a/simulator app/PineLabs_ePOS_Simulator_App_Test_Cases.xlsx
+++ b/simulator app/PineLabs_ePOS_Simulator_App_Test_Cases.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$45</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$J$40</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="211">
   <si>
     <t>Test_Id</t>
   </si>
@@ -293,18 +293,6 @@
     <t>{"Header":{"MethodId":"1001","ApplicationId":"1001","UserId":"userId","VersionNo":"1.0"},"Detail":{"HostResponse":"TRANSACTION INITIATED CHECK GET STATUS","MerchantAddress":"OKHLA B 63 INDUSTRIAL AREA PHASE-1 SOUTH","MerchantCity":"Delhi","AcquiringBankCode":"4","PlutusVersion":"v1.0.0","Remark":"TRANSACTION INITIATED CHECK GET STATUS","LoyaltyPointsAwarded":0,"MerchantId":"HDFC000000649003","BillingRefNo":"upi1234","TerminalId":"20020000172","InvoiceNumber":105,"AmountProcessed":"2000","PrintCardholderName":0,"TransactionTime":"001109","PineLabsBatchId":2000,"CardType":"UPI","MerchantName":"PANEX OVERSEASE","TransactionDate":"04082020","PineLabsRoc":5120,"BatchNumber":9007,"AcquirerName":"ICICI UPI"},"Response":{"ParameterJson":"parameter","ResponseCode":100,"AppVersion":"190618","ResponseMsg":"TRANSACTION INITIATED CHECK GET STATUS"}}</t>
   </si>
   <si>
-    <t>HDFC UPI</t>
-  </si>
-  <si>
-    <t>a.App will send Json request b. Epos app invoked. c. Click UPI . d. Click HDFC UPI . e. QR Code displayed on Epos app screen. f. Customer scan the QR code g. Customer do the transaction.</t>
-  </si>
-  <si>
-    <t>{"Detail":{"BankCode":"2","BillingRefNo":"upi1234","PaymentAmount":2000,"TransactionType":5120},"Header":{"ApplicationId":"1001","MethodId":"1001","UserId":"userId","VersionNo":"1.0"}}</t>
-  </si>
-  <si>
-    <t>{"Header":{"MethodId":"1001","ApplicationId":"1001","UserId":"userId","VersionNo":"1.0"},"Detail":{"HostResponse":"TRANSACTION INITIATED CHECK GET STATUS","MerchantAddress":"OKHLA B 63 INDUSTRIAL AREA PHASE-1 SOUTH","MerchantCity":"Delhi","AcquiringBankCode":"2","PlutusVersion":"v1.0.0","Remark":"TRANSACTION INITIATED CHECK GET STATUS","LoyaltyPointsAwarded":0,"MerchantId":"HDFC000000649003","BillingRefNo":"upi1234","TerminalId":"20020000172","InvoiceNumber":105,"AmountProcessed":"2000","PrintCardholderName":0,"TransactionTime":"001109","PineLabsBatchId":2000,"CardType":"UPI","MerchantName":"PANEX OVERSEASE","TransactionDate":"04082020","PineLabsRoc":5120,"BatchNumber":9007,"AcquirerName":"HDFC UPI"},"Response":{"ParameterJson":"parameter","ResponseCode":100,"AppVersion":"190618","ResponseMsg":"TRANSACTION INITIATED CHECK GET STATUS"}}</t>
-  </si>
-  <si>
     <t>UPIVOID_5121_01</t>
   </si>
   <si>
@@ -434,66 +422,9 @@
     <t>{"Header":{"MethodId":"1001","ApplicationId":"1001","UserId":"userId","VersionNo":"1.0"},"Detail":{"HostResponse":"APPROVED","MerchantAddress":"OKHLA B 63 INDUSTRIAL AREA PHASE-1 SOUTH","MerchantCity":"Delhi","AcquiringBankCode":"4","PlutusVersion":"v1.0.0","Remark":"APPROVED","LoyaltyPointsAwarded":0,"MerchantId":"HDFC000000649003","BillingRefNo":"upi1234","TerminalId":"20020000172","InvoiceNumber":106,"AmountProcessed":"2000","RetrievalReferenceNumber":"009900415668","PrintCardholderName":0,"TransactionTime":"001436","ApprovalCode":"000039","CardNumber":"1234****dfcbank","PineLabsBatchId":2000,"CardType":"UPI","MerchantName":"PANEX OVERSEASE","TransactionDate":"04082020","PineLabsRoc":5122,"BatchNumber":9007,"AcquirerName":"ICICI UPI"},"Response":{"ParameterJson":"parameter","ResponseCode":0,"AppVersion":"190618","ResponseMsg":"APPROVED"}}</t>
   </si>
   <si>
-    <t>BHARATQR_5123_01</t>
-  </si>
-  <si>
-    <t>HDFC BQR</t>
-  </si>
-  <si>
-    <t>App will send Json request QR Code genrated on EPOS app. Custmer will scan QR. Casheir will initatate Get status</t>
-  </si>
-  <si>
     <t>TRANSACTION INITIATED CHECK GET STATUS</t>
   </si>
   <si>
-    <t>{"Detail":{"BankCode":"01","BillingRefNo":"bqr1234","PaymentAmount":2500,"TransactionType":5123},"Header":{"ApplicationId":"1001","MethodId":"1001","UserId":"userId","VersionNo":"1.0"}}</t>
-  </si>
-  <si>
-    <t>{"Header":{"MethodId":"1001","ApplicationId":"1001","UserId":"userId","VersionNo":"1.0"},"Detail":{"HostResponse":"TRANSACTION INITIATED CHECK GET STATUS","MerchantAddress":"OKHLA B 63 INDUSTRIAL AREA PHASE-1 SOUTH","MerchantCity":"Delhi","AcquiringBankCode":"1","PlutusVersion":"v1.0.0","Remark":"TRANSACTION INITIATED CHECK GET STATUS","LoyaltyPointsAwarded":0,"MerchantId":"40622913","BillingRefNo":"bqr1234","TerminalId":"40066446","InvoiceNumber":108,"AmountProcessed":"2500","PrintCardholderName":0,"TransactionTime":"001753","PineLabsBatchId":2500,"CardType":"BharatQR","MerchantName":"PANEX OVERSEASE","TransactionDate":"04082020","PineLabsRoc":5123,"BatchNumber":9007,"AcquirerName":"HDFC BHARAT QR"},"Response":{"ParameterJson":"parameter","ResponseCode":100,"AppVersion":"190618","ResponseMsg":"TRANSACTION INITIATED CHECK GET STATUS"}}</t>
-  </si>
-  <si>
-    <t>Verify BharatQR transaction when Transaction is supported on terminal for the merchant</t>
-  </si>
-  <si>
-    <t>1. Perform a BharatQR transaction with Payment Amount = 200 (in Paisa) 2. Click on Print/ Proceed to Feedback on Receipt page 3. Submit/ Skip feedback questions</t>
-  </si>
-  <si>
-    <t>{"Detail":{"BillingRefNo":"TX12345678","PaymentAmount":200,"TransactionType":5123},"Header":{"ApplicationId":"1001","MethodId":"1001","UserId":"***123**123***","VersionNo":"1.0"}}</t>
-  </si>
-  <si>
-    <t>{"Response":{"AppVersion":"123","ResponseMsg":"APPROVED","ResponseCode":0,"ParameterJson":"parameter"},"Header":{"VersionNo":"1.0","ApplicationId":"1001","MethodId":"1001","UserId":"***123**123***"},"Detail":{"MerchantName":"Vinisdsdsd","CardType":"BharatQR","InvoiceNumber":102,"AcquiringBankCode":"1","PlutusVersion":"v1.0.0","AmountProcessed":"200","BillingRefNo":"TX12345678","MerchantId":"H92946","RetrievalReferenceNumber":"814808146119","TransactionTime":"14:12:45","TransactionDate":"07-04-2019","ApprovalCode":"000005","PineLabsBatchId":200,"HostResponse":"APPROVED","PineLabsRoc":12,"LoyaltyPointsAwarded":0,"TerminalId":"41303199","Remark":"APPROVED","AcquirerName":"HDFC BHARAT QR","MerchantCity":"MEERUT","PrintCardholderName":0,"BatchNumber":9025,"MerchantAddress":"Augharnath Mandir  Meerut Cantt  Meerut "}}</t>
-  </si>
-  <si>
-    <t>BHARATQR_5123_02</t>
-  </si>
-  <si>
-    <t>Verify BharatQR transaction when Host is not reachable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Perform a BharatQR transaction with Payment Amount = 10000 (in Paisa) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"Detail":{"BillingRefNo":"TX12345678","PaymentAmount":10000,"TransactionType":5123},"Header":{"ApplicationId":"1001","MethodId":"1001","UserId":"***123**123***","VersionNo":"1.0"}} </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> {"Response":{"ParameterJson":"parameter","AppVersion":"122","ResponseMsg":"CONNECTIVITY FAILURE","ResponseCode":7},"Header":{"UserId":"***123**123***","MethodId":"1001","ApplicationId":"1001","VersionNo":"1.0"},"Detail":{"InvoiceNumber":106,"MerchantCity":"DIBRUGARH","BatchNumber":9121,"PlutusVersion":"v1.0.0","AcquiringBankCode":"5","HostResponse":"CONNECTIVITY FAILURE","TerminalId":"6546556767","AmountProcessed":"10000","BillingRefNo":"TX12345678","LoyaltyPointsAwarded":0,"TransactionDate":"04072019","TransactionTime":"142028","PineLabsBatchId":10000,"PineLabsRoc":5123,"AcquirerName":"AXIS BHARAT QR","Remark":"CONNECTIVITY FAILURE","MerchantId":"037099890608880","MerchantName":"Tatastarbucks Test","MerchantAddress":"Pine Labs Pvt Ltd","CardType":"BharatQR","PrintCardholderName":0}}</t>
-  </si>
-  <si>
-    <t>BHARATQR_5123_03</t>
-  </si>
-  <si>
-    <t>Verify BharatQR transaction when no scanning is done by Mobile</t>
-  </si>
-  <si>
-    <t>1. Perform a BharatQR transaction with Payment Amount = 1800 (in Paisa)</t>
-  </si>
-  <si>
-    <t>{"Detail":{"BillingRefNo":"TX12345678","PaymentAmount":9900,"TransactionType":5123},"Header":{"ApplicationId":"1001","MethodId":"1001","UserId":"***123**123***","VersionNo":"1.0"}}</t>
-  </si>
-  <si>
-    <t>{"Response":{"ParameterJson":"parameter","AppVersion":"122","ResponseMsg":"TRANSACTION INITIATED CHECK GET STATUS","ResponseCode":7},"Header":{"UserId":"***123**123***","MethodId":"1001","ApplicationId":"1001","VersionNo":"1.0"},"Detail":{"InvoiceNumber":107,"MerchantCity":"DIBRUGARH","BatchNumber":9121,"PlutusVersion":"v1.0.0","AcquiringBankCode":"1","HostResponse":"TRANSACTION INITIATED CHECK GET STATUS","TerminalId":"H92944","AmountProcessed":"9900","BillingRefNo":"TX12345678","LoyaltyPointsAwarded":0,"TransactionDate":"04072019","TransactionTime":"142342","PineLabsBatchId":9900,"PineLabsRoc":5123,"AcquirerName":"HDFC BHARAT QR","Remark":"TRANSACTION INITIATED CHECK GET STATUS","MerchantId":"41303197","MerchantName":"Tatastarbucks Test","MerchantAddress":"Pine Labs Pvt Ltd","CardType":"BharatQR","PrintCardholderName":0}}</t>
-  </si>
-  <si>
     <t>SALE_5561_03</t>
   </si>
   <si>
@@ -707,9 +638,6 @@
     <t>Get Status (5122)</t>
   </si>
   <si>
-    <t>Bharat QR (5123)</t>
-  </si>
-  <si>
     <t>Sale (5561)</t>
   </si>
   <si>
@@ -729,6 +657,9 @@
   </si>
   <si>
     <t>Airtel Money (5127)</t>
+  </si>
+  <si>
+    <t>Sr. No.</t>
   </si>
 </sst>
 </file>
@@ -759,7 +690,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -769,6 +700,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -800,7 +737,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -812,6 +749,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1093,1016 +1034,1173 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="35.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="34" style="1" customWidth="1"/>
-    <col min="6" max="6" width="36.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="69.42578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="35.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="34" style="1" customWidth="1"/>
+    <col min="7" max="7" width="36.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="69.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>216</v>
+      <c r="C1" s="2" t="s">
+        <v>192</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>217</v>
+        <v>193</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>218</v>
+        <v>194</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>220</v>
+        <v>196</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="153.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="153.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>221</v>
-      </c>
-      <c r="C2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="4"/>
       <c r="I2" s="4"/>
-    </row>
-    <row r="3" spans="1:9" ht="64.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="J2" s="4"/>
+    </row>
+    <row r="3" spans="1:10" ht="64.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>221</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="4"/>
       <c r="I3" s="4"/>
-    </row>
-    <row r="4" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="J3" s="4"/>
+    </row>
+    <row r="4" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <f t="shared" ref="A4:A40" si="0">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>221</v>
-      </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="4"/>
       <c r="I4" s="4"/>
-    </row>
-    <row r="5" spans="1:9" ht="153.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="J4" s="4"/>
+    </row>
+    <row r="5" spans="1:10" ht="153.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>221</v>
-      </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="G5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="4"/>
       <c r="I5" s="4"/>
-    </row>
-    <row r="6" spans="1:9" ht="141" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" spans="1:10" ht="141" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>221</v>
-      </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="E6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="F6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="G6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="H6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="4"/>
       <c r="I6" s="4"/>
-    </row>
-    <row r="7" spans="1:9" ht="166.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="J6" s="4"/>
+    </row>
+    <row r="7" spans="1:10" ht="166.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>221</v>
-      </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="E7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="F7" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="G7" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="H7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="4"/>
       <c r="I7" s="4"/>
-    </row>
-    <row r="8" spans="1:9" ht="153.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="J7" s="4"/>
+    </row>
+    <row r="8" spans="1:10" ht="153.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>221</v>
-      </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="E8" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="F8" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="G8" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="H8" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H8" s="4"/>
       <c r="I8" s="4"/>
-    </row>
-    <row r="9" spans="1:9" ht="153.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="J8" s="4"/>
+    </row>
+    <row r="9" spans="1:10" ht="153.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>221</v>
-      </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="E9" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="F9" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="G9" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="H9" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H9" s="4"/>
       <c r="I9" s="4"/>
-    </row>
-    <row r="10" spans="1:9" ht="64.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="J9" s="4"/>
+    </row>
+    <row r="10" spans="1:10" ht="64.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>221</v>
-      </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="E10" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="F10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="G10" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="H10" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="H10" s="4"/>
       <c r="I10" s="4"/>
-    </row>
-    <row r="11" spans="1:9" ht="153.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="J10" s="4"/>
+    </row>
+    <row r="11" spans="1:10" ht="153.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="E11" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="F11" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="G11" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="H11" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="H11" s="4"/>
       <c r="I11" s="4"/>
-    </row>
-    <row r="12" spans="1:9" ht="166.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="J11" s="4"/>
+    </row>
+    <row r="12" spans="1:10" ht="166.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="E12" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="F12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="G12" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="H12" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="H12" s="4"/>
       <c r="I12" s="4"/>
-    </row>
-    <row r="13" spans="1:9" ht="166.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" spans="1:10" ht="166.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="E13" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="F13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="G13" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="H13" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="H13" s="4"/>
       <c r="I13" s="4"/>
-    </row>
-    <row r="14" spans="1:9" ht="166.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="J13" s="4"/>
+    </row>
+    <row r="14" spans="1:10" ht="166.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="E14" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="F14" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="G14" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="H14" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="H14" s="4"/>
       <c r="I14" s="4"/>
-    </row>
-    <row r="15" spans="1:9" ht="166.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="J14" s="4"/>
+    </row>
+    <row r="15" spans="1:10" ht="166.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>223</v>
-      </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="E15" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="F15" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="G15" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="H15" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="H15" s="4"/>
       <c r="I15" s="4"/>
-    </row>
-    <row r="16" spans="1:9" ht="141" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="J15" s="4"/>
+    </row>
+    <row r="16" spans="1:10" ht="141" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>223</v>
-      </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="E16" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="F16" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="G16" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="G16" s="5" t="s">
+      <c r="H16" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="H16" s="4"/>
       <c r="I16" s="4"/>
-    </row>
-    <row r="17" spans="1:9" ht="77.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="J16" s="4"/>
+    </row>
+    <row r="17" spans="1:10" ht="77.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>223</v>
-      </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="E17" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="F17" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="G17" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="H17" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="H17" s="4"/>
       <c r="I17" s="4"/>
-    </row>
-    <row r="18" spans="1:9" ht="141" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="J17" s="4"/>
+    </row>
+    <row r="18" spans="1:10" ht="141" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>223</v>
-      </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="E18" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="F18" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="G18" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="H18" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="H18" s="4"/>
       <c r="I18" s="4"/>
-    </row>
-    <row r="19" spans="1:9" ht="166.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="J18" s="4"/>
+    </row>
+    <row r="19" spans="1:10" ht="166.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>223</v>
-      </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="E19" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="F19" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="G19" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="H19" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="H19" s="4"/>
       <c r="I19" s="4"/>
-    </row>
-    <row r="20" spans="1:9" ht="166.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>68</v>
+      <c r="J19" s="4"/>
+    </row>
+    <row r="20" spans="1:10" ht="166.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
+        <f t="shared" si="0"/>
+        <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>223</v>
-      </c>
-      <c r="C20" s="5" t="s">
         <v>88</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>201</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>89</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>90</v>
+        <v>4</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="H20" s="4"/>
+      <c r="H20" s="5" t="s">
+        <v>92</v>
+      </c>
       <c r="I20" s="4"/>
-    </row>
-    <row r="21" spans="1:9" ht="166.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>92</v>
+      <c r="J20" s="4"/>
+    </row>
+    <row r="21" spans="1:10" ht="64.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="C21" s="5" t="s">
         <v>93</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>201</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>94</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>4</v>
+        <v>95</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>95</v>
+        <v>10</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="H21" s="4"/>
+      <c r="H21" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="I21" s="4"/>
-    </row>
-    <row r="22" spans="1:9" ht="64.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>97</v>
+      <c r="J21" s="4"/>
+    </row>
+    <row r="22" spans="1:10" ht="64.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
+        <f t="shared" si="0"/>
+        <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="C22" s="5" t="s">
         <v>98</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>201</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>99</v>
       </c>
       <c r="E22" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F22" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>100</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="H22" s="4"/>
+      <c r="H22" s="5" t="s">
+        <v>102</v>
+      </c>
       <c r="I22" s="4"/>
-    </row>
-    <row r="23" spans="1:9" ht="64.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>102</v>
+      <c r="J22" s="4"/>
+    </row>
+    <row r="23" spans="1:10" ht="64.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="7">
+        <f t="shared" si="0"/>
+        <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="C23" s="5" t="s">
         <v>103</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>201</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>104</v>
       </c>
       <c r="E23" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F23" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>105</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="H23" s="4"/>
+      <c r="H23" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="I23" s="4"/>
-    </row>
-    <row r="24" spans="1:9" ht="64.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+      <c r="J23" s="4"/>
+    </row>
+    <row r="24" spans="1:10" ht="192" x14ac:dyDescent="0.25">
+      <c r="A24" s="7">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="E24" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="E24" s="5" t="s">
-        <v>10</v>
-      </c>
       <c r="F24" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G24" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="G24" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="H24" s="4"/>
+      <c r="H24" s="5" t="s">
+        <v>111</v>
+      </c>
       <c r="I24" s="4"/>
-    </row>
-    <row r="25" spans="1:9" ht="192" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>111</v>
+      <c r="J24" s="4"/>
+    </row>
+    <row r="25" spans="1:10" ht="64.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
+        <f t="shared" si="0"/>
+        <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="C25" s="5" t="s">
         <v>112</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>202</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>113</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>4</v>
+        <v>114</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>114</v>
+        <v>10</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="H25" s="4"/>
+      <c r="H25" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="I25" s="4"/>
-    </row>
-    <row r="26" spans="1:9" ht="64.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+      <c r="J25" s="4"/>
+    </row>
+    <row r="26" spans="1:10" ht="64.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="7">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="B26" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="D26" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="E26" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="F26" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="G26" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="G26" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="H26" s="4"/>
+      <c r="H26" s="5" t="s">
+        <v>102</v>
+      </c>
       <c r="I26" s="4"/>
-    </row>
-    <row r="27" spans="1:9" ht="64.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+      <c r="J26" s="4"/>
+    </row>
+    <row r="27" spans="1:10" ht="64.5" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="D27" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="E27" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="F27" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="G27" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="G27" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="H27" s="4"/>
+      <c r="H27" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="I27" s="4"/>
-    </row>
-    <row r="28" spans="1:9" ht="64.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+      <c r="J27" s="4"/>
+    </row>
+    <row r="28" spans="1:10" ht="166.5" x14ac:dyDescent="0.25">
+      <c r="A28" s="7">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="C28" s="5" t="s">
+      <c r="E28" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="F28" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="E28" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F28" s="5" t="s">
+      <c r="G28" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="G28" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="H28" s="4"/>
+      <c r="H28" s="5" t="s">
+        <v>128</v>
+      </c>
       <c r="I28" s="4"/>
-    </row>
-    <row r="29" spans="1:9" ht="166.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>128</v>
+      <c r="J28" s="4"/>
+    </row>
+    <row r="29" spans="1:10" ht="166.5" x14ac:dyDescent="0.25">
+      <c r="A29" s="7">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>202</v>
       </c>
       <c r="D29" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="G29" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="H29" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+    </row>
+    <row r="30" spans="1:10" ht="64.5" x14ac:dyDescent="0.25">
+      <c r="A30" s="7">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+    </row>
+    <row r="31" spans="1:10" ht="179.25" x14ac:dyDescent="0.25">
+      <c r="A31" s="7">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+    </row>
+    <row r="32" spans="1:10" ht="64.5" x14ac:dyDescent="0.25">
+      <c r="A32" s="7">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+    </row>
+    <row r="33" spans="1:10" ht="166.5" x14ac:dyDescent="0.25">
+      <c r="A33" s="7">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
+    </row>
+    <row r="34" spans="1:10" ht="166.5" x14ac:dyDescent="0.25">
+      <c r="A34" s="7">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+    </row>
+    <row r="35" spans="1:10" ht="166.5" x14ac:dyDescent="0.25">
+      <c r="A35" s="7">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+    </row>
+    <row r="36" spans="1:10" ht="153.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="7">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
+    </row>
+    <row r="37" spans="1:10" ht="77.25" x14ac:dyDescent="0.25">
+      <c r="A37" s="7">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+    </row>
+    <row r="38" spans="1:10" ht="179.25" x14ac:dyDescent="0.25">
+      <c r="A38" s="7">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="F38" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="G29" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-    </row>
-    <row r="30" spans="1:9" ht="166.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="G30" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-    </row>
-    <row r="31" spans="1:9" ht="166.5" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-    </row>
-    <row r="32" spans="1:9" ht="153.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
-    </row>
-    <row r="33" spans="1:9" ht="179.25" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="G33" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="H33" s="4"/>
-      <c r="I33" s="4"/>
-    </row>
-    <row r="34" spans="1:9" ht="166.5" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="G34" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
-    </row>
-    <row r="35" spans="1:9" ht="64.5" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="G35" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
-    </row>
-    <row r="36" spans="1:9" ht="179.25" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="G36" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-    </row>
-    <row r="37" spans="1:9" ht="64.5" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="H37" s="4"/>
-      <c r="I37" s="4"/>
-    </row>
-    <row r="38" spans="1:9" ht="166.5" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="F38" s="5" t="s">
+      <c r="G38" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
+    </row>
+    <row r="39" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A39" s="7">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="D39" s="5" t="s">
         <v>176</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="H38" s="4"/>
-      <c r="I38" s="4"/>
-    </row>
-    <row r="39" spans="1:9" ht="166.5" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>180</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>181</v>
       </c>
       <c r="F39" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="G39" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="G39" s="5" t="s">
+      <c r="H39" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="H39" s="4"/>
       <c r="I39" s="4"/>
-    </row>
-    <row r="40" spans="1:9" ht="166.5" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
+      <c r="J39" s="4"/>
+    </row>
+    <row r="40" spans="1:10" ht="166.5" x14ac:dyDescent="0.25">
+      <c r="A40" s="7">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="B40" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="B40" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="C40" s="5" t="s">
+      <c r="C40" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="D40" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="D40" s="5" t="s">
+      <c r="E40" s="5" t="s">
         <v>186</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>181</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>187</v>
@@ -2110,133 +2208,11 @@
       <c r="G40" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="H40" s="4"/>
+      <c r="H40" s="5" t="s">
+        <v>189</v>
+      </c>
       <c r="I40" s="4"/>
-    </row>
-    <row r="41" spans="1:9" ht="153.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="F41" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="G41" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="H41" s="4"/>
-      <c r="I41" s="4"/>
-    </row>
-    <row r="42" spans="1:9" ht="77.25" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="G42" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H42" s="4"/>
-      <c r="I42" s="4"/>
-    </row>
-    <row r="43" spans="1:9" ht="179.25" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="F43" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="G43" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="H43" s="4"/>
-      <c r="I43" s="4"/>
-    </row>
-    <row r="44" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="G44" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="H44" s="4"/>
-      <c r="I44" s="4"/>
-    </row>
-    <row r="45" spans="1:9" ht="166.5" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="G45" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="H45" s="4"/>
-      <c r="I45" s="4"/>
+      <c r="J40" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>